<commit_message>
Vragen, antwoorden en symptomen worden geparst, alleen nog followUpQuestions
</commit_message>
<xml_diff>
--- a/excelParser/vragen.xlsx
+++ b/excelParser/vragen.xlsx
@@ -1,34 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robert/Desktop/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="24709"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
   <si>
     <t>voorselectievraag 1</t>
   </si>
@@ -241,6 +236,12 @@
   </si>
   <si>
     <t>foto1.jpg; foto2.jpg</t>
+  </si>
+  <si>
+    <t>foto23.jpg</t>
+  </si>
+  <si>
+    <t>foto2323.jpg;foto235.jpg</t>
   </si>
 </sst>
 </file>
@@ -253,6 +254,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -276,10 +278,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -338,7 +343,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -373,7 +378,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -550,7 +555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,7 +569,7 @@
       <selection activeCell="D1" sqref="D1:U1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="4" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.33203125" bestFit="1" customWidth="1"/>
@@ -572,7 +577,7 @@
     <col min="7" max="21" width="3.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="75">
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
@@ -628,7 +633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="D2" t="s">
         <v>67</v>
       </c>
@@ -639,12 +644,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -652,7 +657,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -660,12 +665,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21">
       <c r="B10" t="s">
         <v>4</v>
       </c>
@@ -673,7 +678,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21">
       <c r="B11" t="s">
         <v>5</v>
       </c>
@@ -681,7 +686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21">
       <c r="B12" t="s">
         <v>6</v>
       </c>
@@ -691,25 +696,30 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:U5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="20.6640625" customWidth="1"/>
     <col min="3" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="21" width="3.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="74" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="74">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
@@ -764,7 +774,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>69</v>
       </c>
@@ -772,11 +782,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21">
       <c r="C3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>70</v>
       </c>
       <c r="E3" t="s">
@@ -786,10 +796,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21">
       <c r="C4" t="s">
         <v>48</v>
       </c>
+      <c r="D4" t="s">
+        <v>71</v>
+      </c>
       <c r="H4" t="s">
         <v>25</v>
       </c>
@@ -797,10 +810,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21">
       <c r="C5" t="s">
         <v>49</v>
       </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
       <c r="L5" t="s">
         <v>25</v>
       </c>
@@ -811,107 +827,112 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="B11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
       <c r="B12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="B13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="B14" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="B15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
       <c r="B16" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Parser verwerkt nu alle vragen die antwoorden hebben
</commit_message>
<xml_diff>
--- a/excelParser/vragen.xlsx
+++ b/excelParser/vragen.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="76">
   <si>
     <t>voorselectievraag 1</t>
   </si>
@@ -242,6 +242,15 @@
   </si>
   <si>
     <t>foto2323.jpg;foto235.jpg</t>
+  </si>
+  <si>
+    <t>Antwo394u</t>
+  </si>
+  <si>
+    <t>ajajaja.png</t>
+  </si>
+  <si>
+    <t>weiorj9</t>
   </si>
 </sst>
 </file>
@@ -566,7 +575,7 @@
   <dimension ref="A1:U12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:U1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -706,224 +715,252 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U25"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="4" width="20.83203125" customWidth="1"/>
-    <col min="5" max="21" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="20" width="3.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="74">
+    <row r="1" spans="1:20" ht="74">
+      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="E1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="U1" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
-      <c r="C3" t="s">
+    <row r="3" spans="1:20">
+      <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
       <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s">
         <v>71</v>
       </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="S4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="G4" t="s">
+        <v>25</v>
+      </c>
+      <c r="R4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
       <c r="C5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" t="s">
         <v>72</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="S5" t="s">
         <v>25</v>
       </c>
       <c r="T5" t="s">
         <v>25</v>
       </c>
-      <c r="U5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="B6" t="s">
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:20">
       <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="R8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
-      <c r="B8" t="s">
+    <row r="10" spans="1:20">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
-      <c r="B9" t="s">
+    <row r="11" spans="1:20">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:21">
-      <c r="B10" t="s">
+    <row r="12" spans="1:20">
+      <c r="A12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:21">
-      <c r="B11" t="s">
+    <row r="13" spans="1:20">
+      <c r="A13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:21">
-      <c r="B12" t="s">
+    <row r="14" spans="1:20">
+      <c r="A14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
-      <c r="B13" t="s">
+    <row r="15" spans="1:20">
+      <c r="A15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:21">
-      <c r="B14" t="s">
+    <row r="16" spans="1:20">
+      <c r="A16" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
-      <c r="B15" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
-      <c r="B16" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
-      <c r="B17" t="s">
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
-      <c r="B18" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:2">
-      <c r="B19" t="s">
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
-      <c r="B20" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
-      <c r="B21" t="s">
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
-      <c r="B22" t="s">
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
-      <c r="B23" t="s">
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:2">
-      <c r="B25" t="s">
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>